<commit_message>
Update expected outputs down to zero.xlsx
</commit_message>
<xml_diff>
--- a/hackerrank/expected outputs down to zero.xlsx
+++ b/hackerrank/expected outputs down to zero.xlsx
@@ -32,12 +32,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,9 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,28 +356,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:Y60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:25" ht="15.75">
       <c r="A1" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:25" ht="15.75">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75">
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1">
+        <v>7</v>
+      </c>
+      <c r="S2" s="1">
+        <v>7</v>
+      </c>
+      <c r="T2" s="1">
+        <v>5</v>
+      </c>
+      <c r="U2" s="1">
+        <v>7</v>
+      </c>
+      <c r="V2" s="1">
+        <v>7</v>
+      </c>
+      <c r="W2" s="1">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75">
       <c r="A3" s="1">
         <v>34</v>
       </c>
@@ -378,7 +454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:25" ht="15.75">
       <c r="A4" s="1">
         <v>86</v>
       </c>
@@ -386,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:25" ht="15.75">
       <c r="A5" s="1">
         <v>73</v>
       </c>
@@ -394,7 +470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:25" ht="15.75">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -402,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:25" ht="15.75">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -410,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:25" ht="15.75">
       <c r="A8" s="1">
         <v>87</v>
       </c>
@@ -418,7 +494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:25" ht="15.75">
       <c r="A9" s="1">
         <v>57</v>
       </c>
@@ -426,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:25" ht="15.75">
       <c r="A10" s="1">
         <v>81</v>
       </c>
@@ -434,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:25" ht="15.75">
       <c r="A11" s="1">
         <v>32</v>
       </c>
@@ -442,7 +518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:25" ht="15.75">
       <c r="A12" s="1">
         <v>83</v>
       </c>
@@ -450,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:25" ht="15.75">
       <c r="A13" s="1">
         <v>39</v>
       </c>
@@ -458,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:25" ht="15.75">
       <c r="A14" s="1">
         <v>98</v>
       </c>
@@ -466,7 +542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:25" ht="15.75">
       <c r="A15" s="1">
         <v>89</v>
       </c>
@@ -474,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:25" ht="15.75">
       <c r="A16" s="1">
         <v>86</v>
       </c>
@@ -547,258 +623,258 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>30</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>78</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>78</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>55</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>39</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>42</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>95</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>95</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>25</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>88</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>51</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
-      <c r="A37" s="1">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="A37" s="2">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>93</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>41</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>90</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>34</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>96</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>68</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>81</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>63</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75">
-      <c r="A46" s="1">
-        <v>6</v>
-      </c>
-      <c r="B46" s="1">
+      <c r="A46" s="2">
+        <v>6</v>
+      </c>
+      <c r="B46" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75">
-      <c r="A47" s="1">
-        <v>7</v>
-      </c>
-      <c r="B47" s="1">
+      <c r="A47" s="2">
+        <v>7</v>
+      </c>
+      <c r="B47" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>33</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>26</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>66</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>79</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>4</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>89</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>14</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>33</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>22</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>